<commit_message>
row and column labels added
</commit_message>
<xml_diff>
--- a/public/Map2.xlsx
+++ b/public/Map2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomasschijf/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomasschijf/Documents/GitHub/infainance/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94A727C8-AA19-4449-81E0-44B223A62AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E3DFA3-D165-2148-9610-DEF7A3EC88C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="1000" windowWidth="27840" windowHeight="16340" xr2:uid="{AE543090-CF86-9D4F-919A-25BC12273A2B}"/>
   </bookViews>
@@ -286,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -315,6 +315,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -533,7 +534,7 @@
   <dimension ref="A1:L966"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -729,28 +730,28 @@
         <v>45</v>
       </c>
       <c r="D13" s="10">
-        <f>E13/C13</f>
-        <v>66.666666666666671</v>
-      </c>
-      <c r="E13" s="4">
-        <v>3000</v>
+        <v>40</v>
+      </c>
+      <c r="E13" s="12">
+        <f>D13*C13</f>
+        <v>1800</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="11">
         <f>E13</f>
-        <v>3000</v>
+        <v>1800</v>
       </c>
       <c r="H13" s="11">
-        <f t="shared" ref="H13:J16" si="0">G13</f>
-        <v>3000</v>
+        <f t="shared" ref="H13:J18" si="0">G13</f>
+        <v>1800</v>
       </c>
       <c r="I13" s="11">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>1800</v>
       </c>
       <c r="J13" s="11">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -765,21 +766,24 @@
         <v>40</v>
       </c>
       <c r="E14" s="12">
-        <f t="shared" ref="E14:E18" si="1">D14*C14</f>
+        <f>D14*C14</f>
         <v>20000</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="11">
-        <v>10000</v>
+        <f t="shared" ref="G14:G18" si="1">E14</f>
+        <v>20000</v>
       </c>
       <c r="H14" s="11">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="I14" s="11">
-        <v>10000</v>
+        <f t="shared" si="0"/>
+        <v>20000</v>
       </c>
       <c r="J14" s="11">
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
     </row>
@@ -795,12 +799,12 @@
         <v>55</v>
       </c>
       <c r="E15" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="E15:E18" si="2">D15*C15</f>
         <v>4290</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="11">
-        <f>E15</f>
+        <f t="shared" si="1"/>
         <v>4290</v>
       </c>
       <c r="H15" s="11">
@@ -828,15 +832,16 @@
         <v>35</v>
       </c>
       <c r="E16" s="12">
+        <f t="shared" si="2"/>
+        <v>1925</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="11">
         <f t="shared" si="1"/>
         <v>1925</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="11">
-        <v>0</v>
-      </c>
       <c r="H16" s="11">
-        <f>E16</f>
+        <f t="shared" si="0"/>
         <v>1925</v>
       </c>
       <c r="I16" s="11">
@@ -860,14 +865,26 @@
         <v>30</v>
       </c>
       <c r="E17" s="12">
+        <f t="shared" si="2"/>
+        <v>3750</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="11">
         <f t="shared" si="1"/>
         <v>3750</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
+      <c r="H17" s="11">
+        <f t="shared" si="0"/>
+        <v>3750</v>
+      </c>
+      <c r="I17" s="11">
+        <f t="shared" si="0"/>
+        <v>3750</v>
+      </c>
+      <c r="J17" s="11">
+        <f t="shared" si="0"/>
+        <v>3750</v>
+      </c>
     </row>
     <row r="18" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
@@ -881,18 +898,24 @@
         <v>30</v>
       </c>
       <c r="E18" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
+      <c r="H18" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I18" s="11">
-        <f>E18</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J18" s="11">
-        <f t="shared" ref="J18" si="2">I18</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -904,25 +927,25 @@
       <c r="C19" s="17"/>
       <c r="D19" s="18">
         <f>AVERAGE(D13:D18)</f>
-        <v>42.777777777777779</v>
+        <v>38.333333333333336</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
       <c r="G19" s="19">
         <f t="shared" ref="G19:J19" si="3">SUM(G13:G18)+SUM(G8:G9)</f>
-        <v>17290</v>
+        <v>31765</v>
       </c>
       <c r="H19" s="19">
         <f t="shared" si="3"/>
-        <v>19215</v>
+        <v>31765</v>
       </c>
       <c r="I19" s="19">
         <f t="shared" si="3"/>
-        <v>19215</v>
+        <v>31765</v>
       </c>
       <c r="J19" s="19">
         <f t="shared" si="3"/>
-        <v>106715</v>
+        <v>109265</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -968,24 +991,28 @@
       </c>
       <c r="D22" s="10">
         <f t="shared" ref="D22:D27" si="5">D13*(1-$B$1)</f>
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="E22" s="4">
-        <f t="shared" ref="E22:E27" si="6">D22*C22</f>
-        <v>1800</v>
+        <f>D22*C22</f>
+        <v>1080</v>
       </c>
       <c r="F22" s="1"/>
+      <c r="G22" s="24">
+        <f>E22</f>
+        <v>1080</v>
+      </c>
       <c r="H22" s="11">
-        <f>D22*C22</f>
-        <v>1800</v>
+        <f>G22</f>
+        <v>1080</v>
       </c>
       <c r="I22" s="11">
-        <f t="shared" ref="I22:J27" si="7">H22</f>
-        <v>1800</v>
+        <f t="shared" ref="I22:J22" si="6">H22</f>
+        <v>1080</v>
       </c>
       <c r="J22" s="11">
-        <f t="shared" si="7"/>
-        <v>1800</v>
+        <f t="shared" si="6"/>
+        <v>1080</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1002,18 +1029,24 @@
         <v>24</v>
       </c>
       <c r="E23" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="E23:E27" si="7">D23*C23</f>
         <v>12000</v>
       </c>
       <c r="F23" s="1"/>
+      <c r="G23" s="24">
+        <f t="shared" ref="G23:G27" si="8">E23</f>
+        <v>12000</v>
+      </c>
       <c r="H23" s="11">
-        <v>5000</v>
+        <f t="shared" ref="H23:J23" si="9">G23</f>
+        <v>12000</v>
       </c>
       <c r="I23" s="11">
-        <f t="shared" si="7"/>
-        <v>5000</v>
+        <f t="shared" si="9"/>
+        <v>12000</v>
       </c>
       <c r="J23" s="11">
+        <f t="shared" si="9"/>
         <v>12000</v>
       </c>
     </row>
@@ -1031,20 +1064,24 @@
         <v>33</v>
       </c>
       <c r="E24" s="4">
-        <f t="shared" si="6"/>
-        <v>2574</v>
-      </c>
-      <c r="F24" s="1"/>
-      <c r="H24" s="11">
-        <f t="shared" ref="H24:H27" si="8">D24*C24</f>
-        <v>2574</v>
-      </c>
-      <c r="I24" s="11">
         <f t="shared" si="7"/>
         <v>2574</v>
       </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="24">
+        <f t="shared" si="8"/>
+        <v>2574</v>
+      </c>
+      <c r="H24" s="11">
+        <f t="shared" ref="H24:J24" si="10">G24</f>
+        <v>2574</v>
+      </c>
+      <c r="I24" s="11">
+        <f t="shared" si="10"/>
+        <v>2574</v>
+      </c>
       <c r="J24" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2574</v>
       </c>
     </row>
@@ -1062,21 +1099,24 @@
         <v>21</v>
       </c>
       <c r="E25" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1155</v>
       </c>
       <c r="F25" s="1"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11">
+      <c r="G25" s="24">
         <f t="shared" si="8"/>
         <v>1155</v>
       </c>
+      <c r="H25" s="11">
+        <f t="shared" ref="H25:J25" si="11">G25</f>
+        <v>1155</v>
+      </c>
       <c r="I25" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1155</v>
       </c>
       <c r="J25" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1155</v>
       </c>
     </row>
@@ -1094,21 +1134,24 @@
         <v>18</v>
       </c>
       <c r="E26" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2250</v>
       </c>
       <c r="F26" s="1"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11">
+      <c r="G26" s="24">
         <f t="shared" si="8"/>
         <v>2250</v>
       </c>
+      <c r="H26" s="11">
+        <f t="shared" ref="H26:J26" si="12">G26</f>
+        <v>2250</v>
+      </c>
       <c r="I26" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>2250</v>
       </c>
       <c r="J26" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>2250</v>
       </c>
     </row>
@@ -1126,21 +1169,24 @@
         <v>18</v>
       </c>
       <c r="E27" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F27" s="1"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11">
+      <c r="G27" s="24">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
+      <c r="H27" s="11">
+        <f t="shared" ref="H27:J27" si="13">G27</f>
+        <v>0</v>
+      </c>
       <c r="I27" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J27" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -1154,20 +1200,20 @@
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
       <c r="G28" s="19">
-        <f t="shared" ref="G28:J28" si="9">SUM(G22:G27)</f>
-        <v>0</v>
+        <f t="shared" ref="G28:J28" si="14">SUM(G22:G27)</f>
+        <v>19059</v>
       </c>
       <c r="H28" s="19">
-        <f t="shared" si="9"/>
-        <v>12779</v>
+        <f t="shared" si="14"/>
+        <v>19059</v>
       </c>
       <c r="I28" s="19">
-        <f t="shared" si="9"/>
-        <v>12779</v>
+        <f t="shared" si="14"/>
+        <v>19059</v>
       </c>
       <c r="J28" s="19">
-        <f t="shared" si="9"/>
-        <v>19779</v>
+        <f t="shared" si="14"/>
+        <v>19059</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1192,20 +1238,20 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="22">
-        <f t="shared" ref="G30:J30" si="10">G19-G28</f>
-        <v>17290</v>
+        <f t="shared" ref="G30:J30" si="15">G19-G28</f>
+        <v>12706</v>
       </c>
       <c r="H30" s="22">
-        <f t="shared" si="10"/>
-        <v>6436</v>
+        <f t="shared" si="15"/>
+        <v>12706</v>
       </c>
       <c r="I30" s="22">
-        <f t="shared" si="10"/>
-        <v>6436</v>
+        <f t="shared" si="15"/>
+        <v>12706</v>
       </c>
       <c r="J30" s="22">
-        <f t="shared" si="10"/>
-        <v>86936</v>
+        <f t="shared" si="15"/>
+        <v>90206</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>